<commit_message>
Completed input of data into swo2023_v001.dat
</commit_message>
<xml_diff>
--- a/Data/Catch/JPN_catch.xlsx
+++ b/Data/Catch/JPN_catch.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="86">
   <si>
     <t>CPUE</t>
   </si>
@@ -353,6 +353,18 @@
   </si>
   <si>
     <t>Fleet Number</t>
+  </si>
+  <si>
+    <t>S5_TWN_WCNPO_DWLL_late</t>
+  </si>
+  <si>
+    <t>S6_US_WCNPO_LL_deep</t>
+  </si>
+  <si>
+    <t>S7_US_WCNPO_LL_shallow_early</t>
+  </si>
+  <si>
+    <t>S8_US_WCNPO_LL_shallow_late</t>
   </si>
 </sst>
 </file>
@@ -747,7 +759,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
@@ -1454,6 +1466,27 @@
       <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E21" s="1">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
@@ -1468,6 +1501,27 @@
       <c r="D22" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E22" s="1">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
@@ -1482,6 +1536,27 @@
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E23" s="1">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
@@ -1496,6 +1571,27 @@
       <c r="D24" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E24" s="1">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
@@ -1510,6 +1606,27 @@
       <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E25" s="1">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
@@ -1524,6 +1641,27 @@
       <c r="D26" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E26" s="1">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
@@ -1538,6 +1676,27 @@
       <c r="D27" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E27" s="1">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
@@ -1551,6 +1710,27 @@
       </c>
       <c r="D28" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="E28" s="1">
+        <v>27</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:11">

</xml_diff>

<commit_message>
first build control file
</commit_message>
<xml_diff>
--- a/Data/Catch/JPN_catch.xlsx
+++ b/Data/Catch/JPN_catch.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="87">
   <si>
     <t>CPUE</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>S8_US_WCNPO_LL_shallow_late</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -756,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="L60" sqref="F34:L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
@@ -1760,6 +1763,603 @@
     <row r="32" spans="1:11" ht="18">
       <c r="A32" s="3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12">
+      <c r="F34" s="1">
+        <v>24</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12">
+      <c r="F35" s="1">
+        <v>24</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K35" s="1">
+        <v>2</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12">
+      <c r="F36" s="1">
+        <v>24</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K36" s="1">
+        <v>3</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12">
+      <c r="F37" s="1">
+        <v>15</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>3</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K37" s="1">
+        <v>4</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12">
+      <c r="F38" s="1">
+        <v>24</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K38" s="1">
+        <v>5</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12">
+      <c r="F39" s="1">
+        <v>15</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K39" s="1">
+        <v>6</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12">
+      <c r="F40" s="1">
+        <v>15</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>2</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K40" s="1">
+        <v>7</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12">
+      <c r="F41" s="1">
+        <v>24</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K41" s="1">
+        <v>8</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12">
+      <c r="F42" s="1">
+        <v>15</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>8</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K42" s="1">
+        <v>9</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12">
+      <c r="F43" s="1">
+        <v>15</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K43" s="1">
+        <v>10</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="6:12">
+      <c r="F44" s="1">
+        <v>24</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K44" s="1">
+        <v>11</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="6:12">
+      <c r="F45" s="1">
+        <v>24</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K45" s="1">
+        <v>12</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="6:12">
+      <c r="F46" s="1">
+        <v>24</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K46" s="1">
+        <v>13</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="6:12">
+      <c r="F47" s="1">
+        <v>15</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>8</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K47" s="1">
+        <v>14</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="6:12">
+      <c r="F48" s="1">
+        <v>15</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
+        <v>8</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K48" s="1">
+        <v>15</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="6:12">
+      <c r="F49" s="1">
+        <v>15</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+      <c r="I49" s="1">
+        <v>11</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K49" s="1">
+        <v>16</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="6:12">
+      <c r="F50" s="1">
+        <v>15</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+      <c r="I50" s="1">
+        <v>11</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K50" s="1">
+        <v>17</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="6:12">
+      <c r="F51" s="1">
+        <v>15</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
+        <v>8</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K51" s="1">
+        <v>18</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="6:12">
+      <c r="F52" s="1">
+        <v>24</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K52" s="1">
+        <v>19</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="6:12">
+      <c r="F53" s="1">
+        <v>15</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K53" s="1">
+        <v>20</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="6:12">
+      <c r="F54" s="1">
+        <v>15</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K54" s="1">
+        <v>21</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="6:12">
+      <c r="F55" s="1">
+        <v>15</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K55" s="1">
+        <v>22</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="6:12">
+      <c r="F56" s="1">
+        <v>15</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K56" s="1">
+        <v>23</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="6:12">
+      <c r="F57" s="1">
+        <v>15</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K57" s="1">
+        <v>24</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="6:12">
+      <c r="F58" s="1">
+        <v>15</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K58" s="1">
+        <v>25</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="6:12">
+      <c r="F59" s="1">
+        <v>15</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K59" s="1">
+        <v>26</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="6:12">
+      <c r="F60" s="1">
+        <v>15</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K60" s="1">
+        <v>27</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>